<commit_message>
Adds the feature to generate .xlsx files with information about full professorship advancement
It's possible to generate files for one reseacher or all of them
</commit_message>
<xml_diff>
--- a/conferences_similar.xlsx
+++ b/conferences_similar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:P163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,16 +476,19 @@
       <c r="O1" s="1" t="n">
         <v>13</v>
       </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Joint Meeting on European Software Engineering Conference and Foundations of Software Engineering (FSE/ESEC)</t>
+          <t>European Conference on Machine Learning and Principles and Practice of Knowledge Discovery in Databases (ECML/PKDD)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>International Workshop on Software Configuration Management (SCM), European Software Engineering Conference (ESEC)/Foundations of Software Engineering (FSE)</t>
+          <t>Discovery Challenge 2004 in conjunction with the 8th European Conference on Principles and Practice of Knowledge Discovery in Databases (PKDD)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -501,16 +504,17 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>IEEE Global Communications Conference (GLOBECOM)</t>
+          <t>Joint Meeting on European Software Engineering Conference and Foundations of Software Engineering (FSE/ESEC)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GLOBECOM 2012 2012 IEEE Global Communications Conference</t>
+          <t>International Workshop on Software Configuration Management (SCM), European Software Engineering Conference (ESEC)/Foundations of Software Engineering (FSE)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -526,19 +530,24 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Conference on Communications (ICC)</t>
+          <t>IEEE Global Communications Conference (GLOBECOM)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IEEE International Conference on Communications</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>GLOBECOM 2012 2012 IEEE Global Communications Conference</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>49th Annual IEEE GLOBECOM Technical Conference</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -551,16 +560,17 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Joint Conference on Neural Networks (IJCNN)</t>
+          <t>Hawaii International Conference on System Sciences (HICSS)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>International Joint Conference on Neural Networks (IJCNN)</t>
+          <t>Annual Hawaii International Conference on System Sciences 2015 (HICSS 2015)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -576,16 +586,17 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>ACM Symposium on Applied Computing (SAC)</t>
+          <t>IEEE International Conference on Communications (ICC)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ACM Symposium on Applied Computing</t>
+          <t>IEEE International Conference on Communications</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -601,21 +612,34 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>European Conference on Artificial Intelligence (ECAI)</t>
+          <t>International Conference on Computational Science (ICCS)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Workshop on Configuration (ConfWS), European Conference on Artificial Intelligence (ECAI)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+          <t>Workshop on Bioinformatics Research and Applications in conjunction with the International Conference on Computational Science</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ICCS 2010 - International Conference on Computational Science 2010</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>10th International Conference on Computational Science</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>XVI International Conference on Computational Science 2016 - ICCS 2016</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -626,23 +650,20 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Biometrics (ICB)</t>
+          <t>International Conference on Machine Learning (ICML)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>International Conference and Exhibition on Electricity Distribution</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>International Conference on Biomedical Ontology</t>
-        </is>
-      </c>
+          <t>International Conference on Optimization and Learning (OLA)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -655,19 +676,24 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Computer Communications and Networks (ICCCN)</t>
+          <t>International Conference on Parallel Processing (ICPP)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IEEE Conference on Computer Communications - Student Workshop</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
+          <t>International Euro-Par Parallel Processing Conference</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>International Conference on Parallel Processing Workshop</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -680,16 +706,17 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>IFIP/IEEE International Symposium on Integrated Network Management (IM)</t>
+          <t>International Joint Conference on Artificial Intelligence (IJCAI)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>International Symposium on Knowledge Management/Document Management (ISKM/DM)</t>
+          <t>The 17th Australian Joint Conference on Artificial Intelligence</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -705,23 +732,20 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>International Symposium on Computers and Communications (ISCC)</t>
+          <t>IEEE International Joint Conference on Neural Networks (IJCNN)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2015 20th IEEE Symposium on Computers and Communication (ISCC)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2016 IEEE Symposium on Computers and Communication (ISCC)</t>
-        </is>
-      </c>
+          <t>International Joint Conference on Neural Networks (IJCNN)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -734,23 +758,20 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Requirements Engineering Conference (RE)</t>
+          <t>IEEE International Symposium on Circuits and Systems (ISCAS)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2014 49th International Universities Power Engineering Conference (UPEC)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2019 IEEE PES AsiaPacific Power and Energy Engineering Conference (APPEEC)</t>
-        </is>
-      </c>
+          <t>Fifth IEEE International Symposium and School on Advance Distributed Systems ISSADS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -763,19 +784,24 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Conference on Software Analysis, Evolution and Reengineering (SANER)</t>
+          <t>ACM Symposium on Applied Computing (SAC)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>International Conference on Software Analysis, Evolution and Reengineering (SANER)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
+          <t>ACM Symposium on Applied Computing</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ACM Symposium on Applied Computing (SAC 2014)</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
@@ -788,16 +814,17 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Advances in Computer Entertainment Technology (ACE)</t>
+          <t>SIAM International Conference on Data Mining (SDM)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>International Conference in Advances in Computer Entertainment Technology (ACE)</t>
+          <t>SIAM International Conference on Data Mining</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -813,28 +840,49 @@
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>International Workshop on Cooperative and Human Aspects of Software Engineering (CHASE)</t>
+          <t>IEEE Conference on Computational Intelligence and Games (CIG)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>International Workshop on Comparison and Versioning of Software Models (CVSM), International Conference on Software Engineering (ICSE)</t>
+          <t>II Conference on Computational Interdisciplinary Science (CCIS)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>International Workshop on Software Engineering in Health Care (SEHC), International Conference on Software Engineering (ICSE)</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+          <t>III Conference on Computational Interdisciplinary Science (CCIS 2014)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>III Conference of Computational Interdisciplinary Sciences (CCIS 2014)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>IEEE Conference on Computational Intelligence and Games (CIG 2015)</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>IEEE Symposium on Computacional Intelligence and Games</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>IV Conference of Computational Interdisciplinary Science (CCIS 2016)</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Conference of Computational Interdisciplinary Science (CCIS 2019)</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -842,16 +890,17 @@
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Conference on Computer and Information Technology (CIT)</t>
+          <t>European Conference on Artificial Intelligence (ECAI)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10th IEEE International Conference on Computer and Information Technology</t>
+          <t>Workshop on Configuration (ConfWS), European Conference on Artificial Intelligence (ECAI)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -867,19 +916,24 @@
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Conference on Computer Supported Cooperative Work in Design (CSCWD)</t>
+          <t>ACM SIGCHI Symposium on Engineering Interactive Computing Systems (EICS)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>International Conference on Computer Supported Cooperative Work in Design (CSCWD)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
+          <t>Brazilian Symposia on Games and Digital Entertainment - Computing Short papers track</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Brazilian Symposia on Games and Digital Entertainment - Computing short papers track</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
@@ -892,23 +946,20 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Computational Science and Engineering (CSE)</t>
+          <t>European Signal Processing Conference (EUSIPCO)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2013 5th International Workshop on Software Engineering for Computational Science and Engineering (SECSE)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>International Workshop on Software Engineering for Computational Science and Engineering (SE-CSE)</t>
-        </is>
-      </c>
+          <t>29th European Simulation and Modelling Conference - ESM 2015</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -921,19 +972,24 @@
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>ACM SIGWEB International Symposium on Document Engineering (DOCENG)</t>
+          <t>ACM Symposium on Interactive 3D Graphics and Games (I3D)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ACM Symposium on Document Engineering (DocEng)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
+          <t>20th Symposium on Computer Graphics and Image Processing</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ACM SIGGRAPH Symposium on Interactive 3D Graphics and Games</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
@@ -946,19 +1002,24 @@
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Federated Conference on Computer Science and Information Systems (FedCSIS)</t>
+          <t>International Conference on Biometrics (ICB)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>World Congress on Computer Science, Engineering and Technology Education</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
+          <t>International Conference and Exhibition on Electricity Distribution</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>International Conference on Biomedical Ontology</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
@@ -971,16 +1032,17 @@
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Engineering of Complex Computer (ICECCS)</t>
+          <t>International Conference on Computer Communications and Networks (ICCCN)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>International Conference on Engineering and Computer Education</t>
+          <t>IEEE Conference on Computer Communications - Student Workshop</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -996,16 +1058,17 @@
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Conference on Machine Learning and Applications (ICMLA)</t>
+          <t>IFIP/IEEE International Symposium on Integrated Network Management (IM)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2015 IEEE 14th International Conference on Machine Learning and Applications (ICMLA)</t>
+          <t>International Symposium on Knowledge Management/Document Management (ISKM/DM)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -1021,19 +1084,24 @@
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Web Engineering (ICWE)</t>
+          <t>International Symposium on Computers and Communications (ISCC)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>International Conference on Engineering Optimization</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
+          <t>2015 20th IEEE Symposium on Computers and Communication (ISCC)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2016 IEEE Symposium on Computers and Communication (ISCC)</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
@@ -1046,19 +1114,24 @@
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Information Integration and Web-based Applications &amp; Services (iiWAS)</t>
+          <t>IEEE International Requirements Engineering Conference (RE)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>International Conference on Information Integration and Web-based Applications and Services (iiWAS)</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
+          <t>2014 49th International Universities Power Engineering Conference (UPEC)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2019 IEEE PES AsiaPacific Power and Energy Engineering Conference (APPEEC)</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
@@ -1071,16 +1144,17 @@
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Conference on Information Reuse and Integration (IRI)</t>
+          <t>IEEE International Conference on Software Analysis, Evolution and Reengineering (SANER)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2003 IEEE International Conference on Information Reuse and Integration (IRI 2003)</t>
+          <t>International Conference on Software Analysis, Evolution and Reengineering (SANER)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -1096,20 +1170,29 @@
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>International Symposium on Computer and Information Sciences (ISCIS)</t>
+          <t>International Conference on Advances in Computer Entertainment Technology (ACE)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8th International Symposium on Systems and Information Security</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+          <t>International Conference in Advances in Computer Entertainment Technology (ACE)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>7th International Conference on Advances in Computer Entertainment Technology</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>International Conference on Advances in Computer Entertainment Technology</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
@@ -1121,16 +1204,17 @@
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>International Symposium on Mathematical Morphology (ISMM)</t>
+          <t>IEEE International Conference on Bioinformatics and Biomedicine (BIBM)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>International Symposium on the Management of Industrial and Corporate Knowledge (ISMICK)</t>
+          <t>2008 IEEE International Conference on Bioinformatics and Biomedcine Workshops</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1146,23 +1230,20 @@
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>IEEE Computer Society Annual Symposium on VLSI (ISVLSI)</t>
+          <t>International Conference on Computer Analysis of Images and Patterns (CAIP)</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>the 29th Annual ACM Symposium</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>the 30th Annual ACM Symposium</t>
-        </is>
-      </c>
+          <t>THE 9TH INTERNATIONAL CONFERENCE ON STRUCTURAL ANALYSIS OF ADVANCED MATERIALS ICSAAM 2019</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -1175,23 +1256,20 @@
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>IEEE Conference on Local Computer Networks (LCN)</t>
+          <t>Canadian Conference on Computational Geometry (CCCG)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2012 IEEE 37th Conference on Local Computer Networks (LCN 2012)</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>IEEE Conference on Local Computer Networks</t>
-        </is>
-      </c>
+          <t>14th Western Canadian Conference on Computing Education (WCCCE 2009)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
@@ -1204,19 +1282,24 @@
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>IFIP International Conference on New Technologies, Mobility and Security (NTMS)</t>
+          <t>International Workshop on Cooperative and Human Aspects of Software Engineering (CHASE)</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>IFIP 19th World Computer Congress, TC-6, 5th IFIP International Conference on Network Control and Engineering for QoS, Security and Mobility, WCC-NETCON 2006.</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr"/>
+          <t>International Workshop on Comparison and Versioning of Software Models (CVSM), International Conference on Software Engineering (ICSE)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>International Workshop on Software Engineering in Health Care (SEHC), International Conference on Software Engineering (ICSE)</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -1229,20 +1312,29 @@
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Robocup International Symposium (RoboCup)</t>
+          <t>IEEE International Conference on Computer and Information Technology (CIT)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>the 2016 24th ACM SIGSOFT International Symposium</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+          <t>10th IEEE International Conference on Computer and Information Technology</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>th Annual International Conference on Computer Games, Multimedia and Allied Technology (CGAT 2012)</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>5th Annual International Conference on Computer Games, Multimedia and Allied Technology (CGAT 2012)</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -1254,16 +1346,17 @@
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Theory and Practice of Digital Libraries (TPDL)</t>
+          <t>IEEE International Conference on Computer Supported Cooperative Work in Design (CSCWD)</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>International Conference on the Foundations of Digital Games (FDG)</t>
+          <t>International Conference on Computer Supported Cooperative Work in Design (CSCWD)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -1279,23 +1372,44 @@
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>International Conference on VLSI Design (VLSID)</t>
+          <t>International Conference on Computational Science and Engineering (CSE)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>International Conference on Very Large Data Bases (VLDB)</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+          <t>2013 5th International Workshop on Software Engineering for Computational Science and Engineering (SECSE)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>International Workshop on Software Engineering for Computational Science and Engineering (SE-CSE)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>11th IEEE International Conference on Computational Science and Engineering (CSE-08)</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>5th European Congress on Computational Methods in Applied Sciences and Engineering</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>6TH INTERNATIONAL CONFERENCE ON ADVANCED COMPUTATIONAL ENGINEERING AND EXPERIMENTING, ACE-X 2012</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>6th International Conference on Advanced Computational Engineering and Experimenting ? ACEX2012</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
@@ -1304,16 +1418,17 @@
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>IEEE Wireless Communications and Networking Conference (WCNC)</t>
+          <t>International Conference on Big Data Analytics and Knowledge Discovery (DaWaK)</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>IEEE Blockchain, Robotics and AI for Networking Security Conference</t>
+          <t>6th International Conference on Data Warehousing and Knowledge Discovery</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -1329,16 +1444,17 @@
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Wireless Days Conference (WD)</t>
+          <t>International Conference on Database and Expert Systems Applications (DEXA)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>IFIP Wireless Days Conference</t>
+          <t>2013 24th International Workshop on Database and Expert Systems Applications (DEXA)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -1354,28 +1470,21 @@
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Application of Information and Communication Technologies (AICT)</t>
+          <t>ACM SIGWEB International Symposium on Document Engineering (DOCENG)</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5th International Information and Telecommunicatios Technologies Symposium</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>8th International Information and Telecommunication Technologies Symposium</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>9th International Information and Telecommunication Technologies Symposium</t>
-        </is>
-      </c>
+          <t>ACM Symposium on Document Engineering (DocEng)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
@@ -1387,16 +1496,17 @@
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Annual IEEE Consumer Communications &amp; Networking Conference (CCNC)</t>
+          <t>Federated Conference on Computer Science and Information Systems (FedCSIS)</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2015 12th Annual IEEE Consumer Communications and Networking Conference (CCNC)</t>
+          <t>World Congress on Computer Science, Engineering and Technology Education</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -1412,16 +1522,17 @@
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>International Workshop on Feature-Oriented Software Development (FOSD)</t>
+          <t>International Conference on Computer Graphics Theory and Applications (GRAPP)</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Latin American Workshop on Aspect-Oriented Software Development (LA-WASP)</t>
+          <t>Internacional Conference On Computer Graphics Theory and Application - GRAPP</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -1437,16 +1548,17 @@
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Global Information Infrastructure and Networking Symposium (GIIS)</t>
+          <t>International Conference on Computational Science and Its Applications (ICCSA)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2012 Global Information Infrastructure and Networking Symposium (GIIS)</t>
+          <t>International Conference on Computational Science and its Applications</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -1462,19 +1574,24 @@
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Europe - IEEE International Conference on Innovative Smart Grid Technologies (ISGT-Europe)</t>
+          <t>IFIP International Conference on Entertainment Computing (ICEC)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2015 IEEE PES Innovative Smart Grid Technologies Latin America (ISGT LATAM)</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr"/>
+          <t>IFIP International Conference on Entertainment Computing</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>14th International Conference on Entertainment Computing (ICEC 2015)</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
@@ -1487,16 +1604,17 @@
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Information Technology Based Higher Education and Training (ITHET)</t>
+          <t>International Conference on Engineering of Complex Computer (ICECCS)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2015 IEEE International Conference on Computer and Information Technology; Ubiquitous Computing and Communications; Dependable, Autonomic and Secure Computing; Pervasive Intelligence and Computing (CIT/IUCC/DASC/PICOM)</t>
+          <t>International Conference on Engineering and Computer Education</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -1512,16 +1630,17 @@
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>IEEE Latin-American Conference on Communications (LATINCOM)</t>
+          <t>International Computer Music Conference (ICMC)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8th IEEE Latin-American Conference on Communications</t>
+          <t>International Computer Vision Summer School, 2012</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -1537,19 +1656,24 @@
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Latin American Test Workshop (LATW)</t>
+          <t>IEEE International Conference on Machine Learning and Applications (ICMLA)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>12th IEEE Latin American Test Workshop</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr"/>
+          <t>2015 IEEE 14th International Conference on Machine Learning and Applications (ICMLA)</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>International Conference on Machine Learning and Applications (ICMLA)</t>
+        </is>
+      </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
@@ -1562,16 +1686,17 @@
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Network of the Future (NOF)</t>
+          <t>International Conference on Semantic Computing (ICSC)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7th International Conference on Network of the Future</t>
+          <t>18th International Society of Magnetic Resonance Meeting (ISMAR)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -1587,16 +1712,17 @@
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Power Systems Computation Conference (PSCC)</t>
+          <t>International Conference on Web Engineering (ICWE)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Parallel Computational Fluid Dynamics (ParCFD)</t>
+          <t>International Conference on Engineering Optimization</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -1612,16 +1738,17 @@
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Quality of Information and Communications Technology (QUATIC)</t>
+          <t>International Conference on Information Integration and Web-based Applications &amp; Services (iiWAS)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>International Conference on the Quality of Information and Communications Technology (QUATIC)</t>
+          <t>International Conference on Information Integration and Web-based Applications and Services (iiWAS)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -1637,38 +1764,23 @@
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Banco de Dados (SBBD)</t>
+          <t>IEEE International Conference on Information Reuse and Integration (IRI)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Sessão de Demos do Simpósio Brasileiro de Banco de Dados (SBBD)</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Banco de Dados (SBBD) - Tutorial</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Sessão de Demos do Simpósio Brasileiro de Banco de Dados</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Banco de Dados, Sessão de Pôsteres</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Workshop de Teses e Dissertações do Simpósio Brasileiro de Bancos de Dados (WTDBD)</t>
-        </is>
-      </c>
+          <t>2003 IEEE International Conference on Information Reuse and Integration (IRI 2003)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr"/>
@@ -1678,23 +1790,20 @@
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Brazilian Symposium on Software Engineering (SBES)</t>
+          <t>International Symposium on Computer and Information Sciences (ISCIS)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2011 Brazilian Symposium on Games and Digital Entertainment (SBGAMES)</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>2014 Brazilian Symposium on Software Engineering (SBES)</t>
-        </is>
-      </c>
+          <t>8th International Symposium on Systems and Information Security</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
@@ -1707,23 +1816,20 @@
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Brazilian Symposium on Computing System Engineering (SBESC)</t>
+          <t>International Symposium on Mathematical Morphology (ISMM)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2017 16th Brazilian Symposium on Computer Games and Digital Entertainment (SBGames)</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>2018 17th Brazilian Symposium on Computer Games and Digital Entertainment (SBGames)</t>
-        </is>
-      </c>
+          <t>International Symposium on the Management of Industrial and Corporate Knowledge (ISMICK)</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
@@ -1736,23 +1842,20 @@
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Jogos e Entretenimento Digital (SBGames)</t>
+          <t>International Symposium on Parallel and Distributed Computing (ISPDC)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Games e Entretenimento Digital (SBGames)</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Jogos e Entretenimento Digital (SBGames), Concurso de Teses e Dissertações (CTD)</t>
-        </is>
-      </c>
+          <t>VII Brazilian Symposium of Games and Digital Entertainment - Computing Track</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
@@ -1765,38 +1868,27 @@
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Redes de Computadores e Sistemas Distribuídos (SBRC)</t>
+          <t>IEEE Computer Society Annual Symposium on VLSI (ISVLSI)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>13 o Simpósio Brasileiro de Redes de Computadores</t>
+          <t>the 29th Annual ACM Symposium</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Redes de Computadores</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Redes de Computadores e Sistemas Distribuídos</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Workshop de Redes de Acesso, em conjunto com Simpósio Brasileiro de Redes de Computadores e Sistemas Distribuídos</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Salão de Ferramentas do Simpósio Brasileiro de Redes de Computadores e Sistemas Distribuídos</t>
-        </is>
-      </c>
+          <t>the 30th Annual ACM Symposium</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
@@ -1806,28 +1898,21 @@
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Brazilian Symposium on Bioinformatics (BSB)</t>
+          <t>International Conference on Information Technology : New Generations (ITNG)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>the 30th Brazilian Symposium</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>the XXXIII Brazilian Symposium</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>the IV Brazilian Symposium</t>
-        </is>
-      </c>
+          <t>VII Congresso de Inovação Tecnológica em Energia Elétrica (CITENEL)</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
@@ -1839,33 +1924,30 @@
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Conferencia Latinoamericana de Informática (CLEI)</t>
+          <t>International Conference on Systems, Signals and Image Processing (IWSSIP)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>XXXIII Conferencia Latinoamericana de Informática</t>
+          <t>15th International Conference on Systems, Signals and Image Processing, IWSSIP 2008</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>XXXVI Conferência Latino-americana de Informática</t>
+          <t>16th International Workshop on Systems, Signals and Image Processing</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Encuentro Regional Iberoamericano de Cigré</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Conferência Latino-americana de Informática (CLEI)</t>
-        </is>
-      </c>
+          <t>IWSSIP 2010 - 17th International Conference on Systems, Signals and Image Processing</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
@@ -1876,19 +1958,24 @@
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Annual Simulation and AI in Games Conference (GAMEON)</t>
+          <t>IEEE Conference on Local Computer Networks (LCN)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>XVI CLAIO and XLIV SBPO Joint Conference</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr"/>
+          <t>2012 IEEE 37th Conference on Local Computer Networks (LCN 2012)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>IEEE Conference on Local Computer Networks</t>
+        </is>
+      </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
@@ -1901,16 +1988,17 @@
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Latin-American Network Operations and Management Symposium (LANOMS)</t>
+          <t>ACM Siggraph Conference on Motion in Games (MIG)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5th Latin American Network Operations and Management Symposium</t>
+          <t>ACM Siggraph Educational Track</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -1926,23 +2014,20 @@
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Brazilian Seminar on Ontologies (ONTOBRAS)</t>
+          <t>IFIP International Conference on New Technologies, Mobility and Security (NTMS)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Seminário de Pesquisa em Ontologia no Brasil (ONTOBRAS)</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Seminário de Pesquisa em Ontologia do Brasil (ONTOBRAS)</t>
-        </is>
-      </c>
+          <t>IFIP 19th World Computer Congress, TC-6, 5th IFIP International Conference on Network Control and Engineering for QoS, Security and Mobility, WCC-NETCON 2006.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
@@ -1955,16 +2040,17 @@
       <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Science and Information Conference (SAICC)</t>
+          <t>ACM SIGSIM Conference on Principles of Advanced Discrete Simulation (PADS)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Database Technologies for Handling XML Information on the Web (DATAX)</t>
+          <t>25th ACM/IEEE/SCS Workshop on Principles of Advanced and Distributed Simulation</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
@@ -1980,23 +2066,20 @@
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Brazilian Symposium on Components, Architectures and Reuse Software (SBCARS)</t>
+          <t>Robocup International Symposium (RoboCup)</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Componentes, Arquiteturas e Reuso de Software (SBCARS)</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>2016 X Brazilian Symposium on Software Components, Architectures and Reuse (SBCARS)</t>
-        </is>
-      </c>
+          <t>the 2016 24th ACM SIGSOFT International Symposium</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
@@ -2009,38 +2092,31 @@
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Computação Musical (SBCM)</t>
+          <t>PAD - International Symposium on Computer Architecture and High Performance Computing (SBAC-PAD)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>13o Simpósio Brasileiro de Telecomunicações</t>
+          <t>Symposium on Computer Architecture and High Performance Computing</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Telecomunicações</t>
+          <t>III Workshop em Sistemas Computacionais de Alto Desempenho (WSCAD) em conjunto com o Symposium on Computer Architecture and High Performance Computing (SBAC-PAD)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>XXX Simpósio Brasileiro de Telecomunicações</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>XXXI Simpósio Brasileiro de Telecomunicações</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Computação Aplicada à Saúde</t>
-        </is>
-      </c>
+          <t>X Simpósio em Sistemas Computacionais (WSCAD-SSC) realizado em conjunto com o 21st Symposium on Computer Architecture and High Performance Computing (SBAC-PAD)</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
@@ -2050,96 +2126,50 @@
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
+          <t>Simpósio Brasileiro de Informática na Educação (SBIE)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Engenharia de Software (SBES), Sessão de Ferramentas</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Engenharia de Software, Sessão de Ferramentas</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Workshop de Teses e Dissertações (WTES), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Workshop de Manutenção de Software Moderna (WMSWM), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Concurso de Teses e Dissertações em Qualidade de Software (CTD-QS), Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Workshop de Teses e Dissertações em Qualidade de Software (WTDQS), Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Componentes, Arquiteturas e Reutilização de Software (SBCARS), Sessão de Ferramentas</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>Workshop de Desenvolvimento Rápido de Aplicações (WDRA), Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>Workshop Brasileiro de e-Science (e-Science), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>Fórum em Educação de Engenharia de Software (FEES), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>Workshop Brasileiro de Visualização de Software (WBVS)</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>Concurso de Teses e Dissertações em Qualidade de Software (CTDQS), Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
-        </is>
-      </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Componentes, Arquitetura e Reutilização de Software (SBCARS)</t>
-        </is>
-      </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Componentes, Arquiteturas e Reutilização de Software (SBCARS)</t>
-        </is>
-      </c>
+          <t>XIX Simpósio Brasileiro de Informática na Educação (SBIE 2008)</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Sistemas Colaborativos (SBSC)</t>
+          <t>International Conference on Software Engineering and Knowledge Engineering (SEKE)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>XII Simpósio Brasileiro de Sistemas Multimídia e Web</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr"/>
+          <t>XXV International Conference on Software Engineering &amp; Knowledge Engineering (SEKE 2013)</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>International Conference on Software Engineering and Knowledge Engineering (SEKE 2014)</t>
+        </is>
+      </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
@@ -2152,23 +2182,20 @@
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro em Segurança da Informação e de Sistemas Computacionais (SBSeg)</t>
+          <t>Conference on Graphics, Patterns and Images (SIBGRAPI)</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>XIII Simpósio Brasileiro em Segurança da Informação e de Sistemas Computacionais</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Engenharia de Sistemas Computacionais</t>
-        </is>
-      </c>
+          <t>SIBGRAPI 2013 - XXV Conference on Graphics, Patterns and Images</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
@@ -2181,16 +2208,17 @@
       <c r="M62" t="inlineStr"/>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>Workshop on Social and Human Aspects of Business Process Management (BPMS2)</t>
+          <t>International Conference on Theory and Practice of Digital Libraries (TPDL)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Workshop Anual do MPS (WAMPS), Sessão de Ferramentas</t>
+          <t>International Conference on the Foundations of Digital Games (FDG)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
@@ -2206,23 +2234,20 @@
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Brazilian e-Science Workshop (BRESCI)</t>
+          <t>International Conference on VLSI Design (VLSID)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>eScience Workshop</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Challenges in eScience Workshop (CIS)</t>
-        </is>
-      </c>
+          <t>International Conference on Very Large Data Bases (VLDB)</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
@@ -2235,16 +2260,17 @@
       <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Workshop on Computational Linguistics for Linguistic Complexity (CL4LC)</t>
+          <t>IEEE Virtual Reality Conference (VR)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Workshop Emerging Computational Methods for the Life Sciences (ECMLS)</t>
+          <t>IV workshop e-Science of the Brazilian Society Conference</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -2260,20 +2286,29 @@
       <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>IEEE International Conference on Dependable Systems and Networks Workshops (DSNW)</t>
+          <t>Vehicular Technology Conference (VTC)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2019 22nd Conference on Innovation in Clouds, Internet and Networks and Workshops (ICIN)</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
+          <t>GPU Technology Conference 2013</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>GPU Technology Conference 2014 (GTC 2014)</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>GPU Technology Conference 2015 (GTC 2015)</t>
+        </is>
+      </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
@@ -2285,16 +2320,17 @@
       <c r="M66" t="inlineStr"/>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Encontro Nacional de Inteligencia Artificial e Computacional (ENIAC)</t>
+          <t>IEEE Wireless Communications and Networking Conference (WCNC)</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Encontro Nacional de Informática Aplicada ao Legislativo (ENIAL)</t>
+          <t>IEEE Blockchain, Robotics and AI for Networking Security Conference</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
@@ -2310,16 +2346,17 @@
       <c r="M67" t="inlineStr"/>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>Workshop Latinoamericano de Ingeniería de Software Experimental (ESELAW)</t>
+          <t>Wireless Days Conference (WD)</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Workshop Iberoamericano de Ingeniería de Requisitos y Ambientes de Software (IDEAS)</t>
+          <t>IFIP Wireless Days Conference</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -2335,16 +2372,17 @@
       <c r="M68" t="inlineStr"/>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>International Workshop on Green and Sustainable Software (GREENS)</t>
+          <t>IAT - IEEE/WIC/ACM International Conference on Web Intelligence and Intelligent Agent Technology (WI-IAT)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>NSF-sponsored workshop on Studying Professional Software Design</t>
+          <t>2014 IEEE/WIC/ACM International Joint Conferences on Web Intelligence (WI) and Intelligent Agent Technologies (IAT)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -2360,16 +2398,17 @@
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>International Workshop on High Performance Computing on Bioinformatics (HPCB)</t>
+          <t>International conference on Cellular Automata for Research and Industry (ACRI)</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>International Workshop on High-Performance Data Management in Grid Environments</t>
+          <t>International Conference on Cellular Automata for Research and Industry</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -2385,20 +2424,29 @@
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>CCI - Latin American Conference on Computational Intelligence (LA-CCI)</t>
+          <t>International Conference on Application of Information and Communication Technologies (AICT)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Congresso Ibero-Latino-Americano de Métodos Computacionais em Engenharia (CILAMCE)</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+          <t>5th International Information and Telecommunicatios Technologies Symposium</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>8th International Information and Telecommunication Technologies Symposium</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>9th International Information and Telecommunication Technologies Symposium</t>
+        </is>
+      </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
@@ -2410,19 +2458,24 @@
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>IEEE Workshop on Managing Ubiquitous Communications and Services (MUCS)</t>
+          <t>Annual IEEE Consumer Communications &amp; Networking Conference (CCNC)</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Workshop on Many-Task Computing on Grids and Supercomputers (MTAGS)</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr"/>
+          <t>2015 12th Annual IEEE Consumer Communications and Networking Conference (CCNC)</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>IEEE Consumer Communications and Networking Conference - CCNC 2015</t>
+        </is>
+      </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
@@ -2435,23 +2488,20 @@
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Pesquisa Operacional (SBPO)</t>
+          <t>Conference on Online Social Networks (COSN)</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>XL Simpósio Brasileiro de Pesquisa Operacional</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Simpósio Brasileiro de Pesquisa Operacional</t>
-        </is>
-      </c>
+          <t>Conferencia de Ciências e Artes dos Videojogos</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
@@ -2464,16 +2514,17 @@
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>Seminário Integrado de Software e Hardware (SEMISH)</t>
+          <t>European Control Conference (ECC)</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>XL Seminário Integrado de Software e Hardware</t>
+          <t>GAME-ON - European GAME-ON Conference</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
@@ -2489,19 +2540,24 @@
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>IEEE PES Transmission &amp; Distribution Conference and Exposition Latin America (T&amp;DLA)</t>
+          <t>International Workshop on Feature-Oriented Software Development (FOSD)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>IEEE PES Transmission and Distribution Conference and Exposition Latin America</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr"/>
+          <t>Latin American Workshop on Aspect-Oriented Software Development (LA-WASP)</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Primer Workshop Argentino sobre Videojuegos</t>
+        </is>
+      </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
@@ -2514,16 +2570,17 @@
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>International CAD Conference (CAD)</t>
+          <t>Global Information Infrastructure and Networking Symposium (GIIS)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>the 22nd International ACM Conference</t>
+          <t>2012 Global Information Infrastructure and Networking Symposium (GIIS)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
@@ -2539,20 +2596,29 @@
       <c r="M76" t="inlineStr"/>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>Workshop de Desafios da Computação Aplicada à Educação (DesafIE)</t>
+          <t>International Conference on Grid And Pervasive Computing (GPC)</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Escola Regional de Computação Aplicada à Saúde</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
+          <t>International Conference on Metaheuristics and Nature Inspired Computing (META)</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>3rd International Conference on Metaheuristics and Nature Inspired Computing (META)</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>International Conference on Metaheuristics and Nature Inspired Computing</t>
+        </is>
+      </c>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
@@ -2564,16 +2630,17 @@
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>IARIA International Conference on Smart Grids, Green Communications and IT Energy-aware Technologies (ENERGY)</t>
+          <t>International Workshop on Hybrid Metaheuristics (HM)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Third International Conference on Smart Grids, Green Communications and IT Energy-aware Technologies</t>
+          <t>Workshop on HYBRID METAHEURISTICS</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
@@ -2589,16 +2656,17 @@
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>International Workshop on Future Internet and Smart Networks (FINS)</t>
+          <t>Ibero-American Conference on Artificial Intelligence (IBERAMIA)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2º Workshop do testbed FIBRE - Future Internet Brazilian Environment for Experimentation</t>
+          <t>14th IBERAMIA - Ibero-American Conference on Artificial Intelligence</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
@@ -2614,16 +2682,17 @@
       <c r="M79" t="inlineStr"/>
       <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>Workshop on High Performance and Programmable Networking (HPPN)</t>
+          <t>International Conference on Enterprise Information Systems (ICEIS)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>SPIE's Performance and Control of Network Systems II</t>
+          <t>International Conference on Enterprise Information Systems</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -2639,16 +2708,17 @@
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>IARIA International Conference on Networks (ICN)</t>
+          <t>Europe - IEEE International Conference on Innovative Smart Grid Technologies (ISGT-Europe)</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>IADIS International Conference on WWW/Internet</t>
+          <t>2015 IEEE PES Innovative Smart Grid Technologies Latin America (ISGT LATAM)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -2664,16 +2734,17 @@
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>International Conference on Internet Computing and Internet of Things (ICOMP)</t>
+          <t>International Conference on Information Technology Based Higher Education and Training (ITHET)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2020 4th Conference on Cloud and Internet of Things (CIoT)</t>
+          <t>2015 IEEE International Conference on Computer and Information Technology; Ubiquitous Computing and Communications; Dependable, Autonomic and Secure Computing; Pervasive Intelligence and Computing (CIT/IUCC/DASC/PICOM)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -2689,16 +2760,17 @@
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>International Workshop on Confluence (IWC)</t>
+          <t>International Workshop on Combinatorial Algorithms (IWOCA)</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>International Workshop on Challenges in e-Science (CIS)</t>
+          <t>4th International Workshop on Efficient and Experimental Algorithms (WEA)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -2714,16 +2786,17 @@
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>Iberchip Workshop (IWS)</t>
+          <t>IEEE Latin-American Conference on Communications (LATINCOM)</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>IEEE Packet Video Workshop</t>
+          <t>8th IEEE Latin-American Conference on Communications</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -2739,33 +2812,22 @@
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>International Workshop on Science Gateways (IWSG)</t>
+          <t>Latin American Test Workshop (LATW)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>International Workshop on Scientific Workflows (SWF)</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>International Workshop on the Web and Databases (WebDB)</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>International Workshop on Scientific Workflows, SWF</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>International Workshop on Genomic Databases (IWGD)</t>
-        </is>
-      </c>
+          <t>12th IEEE Latin American Test Workshop</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
@@ -2776,23 +2838,20 @@
       <c r="M85" t="inlineStr"/>
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>Metaheuristics International Conference (MIC)</t>
+          <t>International Conference on Network of the Future (NOF)</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>the 18th ACM International Conference</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>the 20th ACM International Conference</t>
-        </is>
-      </c>
+          <t>7th International Conference on Network of the Future</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
@@ -2805,16 +2864,17 @@
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Automação Inteligente (SBAI)</t>
+          <t>International Conference on Operations Research (OR)</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Simpósio Brasileiro de Telecomunicações e Processamento de Sinais</t>
+          <t>International Conference on the Entity-Relationship Approach</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -2830,23 +2890,20 @@
       <c r="M87" t="inlineStr"/>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>Congresso Brasileiro de Agroinformática (SBIAGRO)</t>
+          <t>Power Systems Computation Conference (PSCC)</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>13 Congresso da Sociedade Brasleiro de Computação</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>XXI Congresso Brasileiro de Automática</t>
-        </is>
-      </c>
+          <t>Parallel Computational Fluid Dynamics (ParCFD)</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
@@ -2859,23 +2916,20 @@
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>International Workshop on Theory and Practice of Provenance (TaPP)</t>
+          <t>International Conference on Quality of Information and Communications Technology (QUATIC)</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>USENIX Workshop on the Theory and Practice of Provenance (TaPP)</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>International Workshop on Theory and Practice of Provenance (TAPP)</t>
-        </is>
-      </c>
+          <t>International Conference on the Quality of Information and Communications Technology (QUATIC)</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
@@ -2888,56 +2942,98 @@
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>Congreso Internacional de Informática Educativa (TISE)</t>
+          <t>Simpósio Brasileiro de Banco de Dados (SBBD)</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Minicurso da V Escola Regional de Informática RJ/ES</t>
+          <t>Sessão de Demos do Simpósio Brasileiro de Banco de Dados (SBBD)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>XXVI Concurso de Trabalhos de Iniciação Científica</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr"/>
-      <c r="I90" t="inlineStr"/>
+          <t>Simpósio Brasileiro de Banco de Dados (SBBD) - Tutorial</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Sessão de Demos do Simpósio Brasileiro de Banco de Dados</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Banco de Dados, Sessão de Pôsteres</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Workshop de Teses e Dissertações do Simpósio Brasileiro de Bancos de Dados (WTDBD)</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>II Workshop de Banco de Dados Não Convencionais</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>VII Simpósio Brasileiro de Banco de Dados</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Workshop de Algoritmos de Mineração de Dados, em conjunto com o XX Simpósio Brasileiro de Banco de Dados</t>
+        </is>
+      </c>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>Workshop on Software Visualization, Evolution and Maintenance (VEM)</t>
+          <t>Brazilian Symposium on Software Engineering (SBES)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Workshop Brasileiro de Visualização, Evolução e Manutenção de Software (VEM)</t>
+          <t>2011 Brazilian Symposium on Games and Digital Entertainment (SBGAMES)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Workshop de Visualização, Manutenção e Evolução de Software (VEM)</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr"/>
+          <t>2014 Brazilian Symposium on Software Engineering (SBES)</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Brazilian Symposia on Games and Digital Entertainment</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Brazilian Symposia on Games and Digital Entertainment - Computing Short papers</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>VII Brazilian Symposium of Games and Digital Entertainment</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>XII Brazilian Symposium on Games and Digital Entertainment - SBGames 2013</t>
+        </is>
+      </c>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr"/>
@@ -2946,96 +3042,171 @@
       <c r="M91" t="inlineStr"/>
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>Workshop de Desenvolvimento Distribuído de Software (WDES)</t>
+          <t>Brazilian Symposium on Computing System Engineering (SBESC)</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Workshop de Desenvolvimento Baseado em Componentes (WDBC)</t>
+          <t>2017 16th Brazilian Symposium on Computer Games and Digital Entertainment (SBGames)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Workshop de Desenvolvimento Distribuído de Software (WDDS), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
+          <t>2018 17th Brazilian Symposium on Computer Games and Digital Entertainment (SBGames)</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Workshop de Teses e Dissertações em Qualidade de Software (WTDQS)</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
-      <c r="I92" t="inlineStr"/>
-      <c r="J92" t="inlineStr"/>
-      <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
+          <t>IX Brazilian Symposium on Computer Games and Digital Entertainment</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>X Brazilian Symposium on Computer Games and Digital Entertainment, SBGames 2011 - Computing Track</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>X Brazilian Symposium on Computer Games and Digital Entertainment, SBGames 2011</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>X Brazilian Symposium on Computer Games and Digital Entertainment, SBGames 2011 - Culture Track</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2014 Brazilian Symposium on Computer Games and Digital Entertainment (SBGAMES)</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2015 14th Brazilian Symposium on Computer Games and Digital Entertainment (SBGames)</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>2019 18th Brazilian Symposium on Computer Games and Digital Entertainment (SBGames)</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>XIX Brazilian Symposium on Computer Games and Digital Entertainment (SBgames 2020)</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>XIX Brazilian Symposium on Computer Games and Digital Entertainment (SBGames 2020)</t>
+        </is>
+      </c>
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>Workshop sobre Ensino de IHC (WEIHC)</t>
+          <t>Simpósio Brasileiro de Jogos e Entretenimento Digital (SBGames)</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Workshop Brasileiro de e-Science (e-Science)</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
-      <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr"/>
-      <c r="N93" t="inlineStr"/>
-      <c r="O93" t="inlineStr"/>
+          <t>Simpósio Brasileiro de Games e Entretenimento Digital (SBGames)</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Jogos e Entretenimento Digital (SBGames), Concurso de Teses e Dissertações (CTD)</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>VII Simpósio Brasileiro de Jogos e Entretenimento Digital - SBGames 2008 - Computing Track - Full Papers</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>VII Simpósio Brasileiro de Jogos e Entretenimento Digital - SBGames 2008 - - Computing Track - Full Papers</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>VIII Simpósio Brasileiro de Jogos e Entretenimento Digital - Full papers Computing Track</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>VIII Simpósio Brasileiro de Jogos e Entretenimento Digital - Computing - Tecnical Posters</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>VIII Simpósio Brasileiro de Jogos e Entretenimento Digital - Computing - Full Papers</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>VIII Simpósio Brasileiro de Jogos e Entretenimento Digital - Computing Technical Poster</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>VIII Simpósio Brasileiro de Jogos e Entretenimento Digital - Computing / Short Papers</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>VIII Simpósio Brasileiro de Jogos e Entretenimento Digital - Track Educação e Cultura</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>XI Simpósio Brasileiro de Jogos e Entretenimento Digital (SBGames 2012)</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>XIII SBGames - Simpósio Brasileiro de Jogos e Entretenimento Digital - SBGAMES 2014</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>XIII SBGames - Simpósio Brasileiro de Jogos e Entretenimento Digital - SBGAMES 2014 (Art and Design Track)</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Jogos e Entretenimento Digital (SBGAMES 2016)</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>XVI Simposio Brasileiro de Jogos e Entretenimento Digital (SBGames 2017)</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>Workshop de Engenharia de Software Baseada em Busca (WESB)</t>
+          <t>Brazilian Symposium on Artificial Intelligence (SBIA)</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>XV Workshop de Gerência e Operação de Redes e Serviços</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Workshop de Gerência e Operação de Redes e Serviços</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>XVII Workshop de Gerência e Operação de Redes e Serviços</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>Workshop de Manutenção de Software Moderna (WMSWM)</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>Workshop de Teses e Dissertações em Engenharia de Software (WTES), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
-        </is>
-      </c>
+          <t>Concurso de Teses e Dissertações em Inteligência Artificial (CTDIA), em conjunto com o 19th Brazilian Symposium on Artificial Intelligence (SBIA)</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr"/>
@@ -3045,22 +3216,39 @@
       <c r="M94" t="inlineStr"/>
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>Workshop de Ferramentas e Aplicações (WFA)</t>
+          <t>Simpósio Brasileiro de Redes de Computadores e Sistemas Distribuídos (SBRC)</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Salão de Ferramentas do SBRC</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr"/>
+          <t>13 o Simpósio Brasileiro de Redes de Computadores</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Redes de Computadores</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Redes de Computadores e Sistemas Distribuídos</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Workshop de Redes de Acesso, em conjunto com Simpósio Brasileiro de Redes de Computadores e Sistemas Distribuídos</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Salão de Ferramentas do Simpósio Brasileiro de Redes de Computadores e Sistemas Distribuídos</t>
+        </is>
+      </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr"/>
@@ -3070,16 +3258,17 @@
       <c r="M95" t="inlineStr"/>
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>Workshop de Redes P2P, Dinâmicas, Sociais e Orientadas a Conteúdo (WP2P+)</t>
+          <t>Simpósio Brasileiro de Sistemas de Informação (SBSI)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Workshop de Redes Dinamicas e Sistemas Peer-to-Peer (WP2P)</t>
+          <t>Encontro Regional de Computação e Sistemas de Informação 2014</t>
         </is>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -3095,16 +3284,17 @@
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>Workshop de Software Livre (WSL)</t>
+          <t>International Meeting on High Performance Computing for Computational Science (VECPAR)</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Workshop on Software Reuse Efforts (WSRE)</t>
+          <t>VECPAR 2010 - 9th International Meeting on High Performance Computing for Computational Science</t>
         </is>
       </c>
       <c r="C97" t="inlineStr"/>
@@ -3120,28 +3310,21 @@
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>Workshop de Testes e Tolerância a Falhas (WTF)</t>
+          <t>Vision, Modeling &amp; Visualization (VMV)</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Workshop de Teses e Dissertações do CBSoft (WTDSoft)</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Workshop de Teses e Dissertações em Banco de Dados (WTDBD)</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>Concurso de Teses e Dissertações da SBC (CTD)</t>
-        </is>
-      </c>
+          <t>Information Visualization</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="inlineStr"/>
       <c r="G98" t="inlineStr"/>
@@ -3153,6 +3336,2013 @@
       <c r="M98" t="inlineStr"/>
       <c r="N98" t="inlineStr"/>
       <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Brazilian Symposium on Bioinformatics (BSB)</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>the 30th Brazilian Symposium</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>the XXXIII Brazilian Symposium</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>the IV Brazilian Symposium</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Brazilian Symposium on Bioinformatics</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>Conferencia Latinoamericana de Informática (CLEI)</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>XXXIII Conferencia Latinoamericana de Informática</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>XXXVI Conferência Latino-americana de Informática</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Encuentro Regional Iberoamericano de Cigré</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Conferência Latino-americana de Informática (CLEI)</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>European Dependable Computing Conference (EDCC)</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Parallel Computing Conference</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>Eurohaptics (EUROHAPTICS)</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Eurographics</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>Annual Simulation and AI in Games Conference (GAMEON)</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>XVI CLAIO and XLIV SBPO Joint Conference</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Eurosis GAMEON - AI and Simulation in Games Conference</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>GAMEON - AI and Simulation in Games Conference</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr"/>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>Brazilian Symposium on GeoInformatics (GeoInfo)</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>X Brazilian Symposium on GeoInformatics</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>International Conference on Fuzzy Theory and its Applications (IFUZZY)</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>THE SIXTH INTERNATIONAL SCHOOL ON FIELD THEORY AND GRAVITATION2012</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>Latin-American Network Operations and Management Symposium (LANOMS)</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>5th Latin American Network Operations and Management Symposium</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>Brazilian Seminar on Ontologies (ONTOBRAS)</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Seminário de Pesquisa em Ontologia no Brasil (ONTOBRAS)</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Seminário de Pesquisa em Ontologia do Brasil (ONTOBRAS)</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>Science and Information Conference (SAICC)</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Database Technologies for Handling XML Information on the Web (DATAX)</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>Brazilian Symposium on Components, Architectures and Reuse Software (SBCARS)</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Componentes, Arquiteturas e Reuso de Software (SBCARS)</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2016 X Brazilian Symposium on Software Components, Architectures and Reuse (SBCARS)</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2012 Sixth Brazilian Symposium on Software Components, Architectures and Reuse (SBCARS 2012)</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>XXIIth Brazilian Symposium on Computer Graphics and Image Processing</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Computação Musical (SBCM)</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>13o Simpósio Brasileiro de Telecomunicações</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Telecomunicações</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>XXX Simpósio Brasileiro de Telecomunicações</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>XXXI Simpósio Brasileiro de Telecomunicações</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Computação Aplicada à Saúde</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Anais Principais do Simpósio Brasileiro de Computação Aplicada à Saúde</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>II Simpósio Brasileiro de Games - Computing Short papers</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de computação gráfica e processamento de imagens</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Brazilian Symposium on Programming Languages (SBLP)</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>XXIInd Brazilian Symposium on Computer Graphics and Image Processing (Sibgrapi 2009)</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Engenharia de Software (SBES), Sessão de Ferramentas</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Engenharia de Software, Sessão de Ferramentas</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Workshop de Teses e Dissertações (WTES), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Workshop de Manutenção de Software Moderna (WMSWM), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Concurso de Teses e Dissertações em Qualidade de Software (CTD-QS), Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Workshop de Teses e Dissertações em Qualidade de Software (WTDQS), Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Componentes, Arquiteturas e Reutilização de Software (SBCARS), Sessão de Ferramentas</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Workshop de Desenvolvimento Rápido de Aplicações (WDRA), Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>Workshop Brasileiro de e-Science (e-Science), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>Fórum em Educação de Engenharia de Software (FEES), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>Workshop Brasileiro de Visualização de Software (WBVS)</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>Concurso de Teses e Dissertações em Qualidade de Software (CTDQS), Simpósio Brasileiro de Qualidade de Software (SBQS)</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Componentes, Arquitetura e Reutilização de Software (SBCARS)</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Componentes, Arquiteturas e Reutilização de Software (SBCARS)</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>XXI Simpósio Brasileiro de Engenharia de Software</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Sistemas Colaborativos (SBSC)</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>XII Simpósio Brasileiro de Sistemas Multimídia e Web</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro em Segurança da Informação e de Sistemas Computacionais (SBSeg)</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>XIII Simpósio Brasileiro em Segurança da Informação e de Sistemas Computacionais</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Engenharia de Sistemas Computacionais</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>International Conference on Serious Games and Applications for Health (SeGAH)</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>2014 IEEE 3rd International Conference on Serious Games and Applications for Health (SeGAH)</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>IEEE 3rd International Conference on Serious Games and Applications for Health (SEGAH 2014)</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>2016 IEEE International Conference on Serious Games and Applications for Health (SeGAH)</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+      <c r="K115" t="inlineStr"/>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>Workshop sobre Educação em Computação (WEI)</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>XVI Workshop sobre Educação em Computação - WEI 2008</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+      <c r="K116" t="inlineStr"/>
+      <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr"/>
+      <c r="O116" t="inlineStr"/>
+      <c r="P116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>Simpósio em Sistemas Computacionais de Alto Desempenho (WSCAD)</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Simpósio em Sistemas Computacionais (WSCAD-SSC)</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Escola Regional de Alto Desempenho, 2017</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>XVIII Simpósio em Sistemas Computacionais de Alto Desempenho - Workshop de Iniciação Científica, 2017</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr"/>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
+      <c r="K117" t="inlineStr"/>
+      <c r="L117" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
+      <c r="P117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>International Conference in Central Europe on Computer Graphics and Visualization and Computer Vision (WSCG)</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>International Conferences in Central Europe on Computer Graphics, Visualization and Computer Vision</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
+      <c r="K118" t="inlineStr"/>
+      <c r="L118" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" t="inlineStr"/>
+      <c r="O118" t="inlineStr"/>
+      <c r="P118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>Workshop on Social and Human Aspects of Business Process Management (BPMS2)</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Workshop Anual do MPS (WAMPS), Sessão de Ferramentas</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
+      <c r="K119" t="inlineStr"/>
+      <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" t="inlineStr"/>
+      <c r="O119" t="inlineStr"/>
+      <c r="P119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>Brazilian e-Science Workshop (BRESCI)</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>eScience Workshop</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Challenges in eScience Workshop (CIS)</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>VI e-Science Workshop</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>V e-Science Workshop</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
+      <c r="K120" t="inlineStr"/>
+      <c r="L120" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" t="inlineStr"/>
+      <c r="O120" t="inlineStr"/>
+      <c r="P120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>Workshop on Computational Linguistics for Linguistic Complexity (CL4LC)</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Workshop Emerging Computational Methods for the Life Sciences (ECMLS)</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
+      <c r="K121" t="inlineStr"/>
+      <c r="L121" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" t="inlineStr"/>
+      <c r="O121" t="inlineStr"/>
+      <c r="P121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>IEEE International Conference on Dependable Systems and Networks Workshops (DSNW)</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>2019 22nd Conference on Innovation in Clouds, Internet and Networks and Workshops (ICIN)</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
+      <c r="K122" t="inlineStr"/>
+      <c r="L122" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>Encontro Nacional de Inteligencia Artificial e Computacional (ENIAC)</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Encontro Nacional de Informática Aplicada ao Legislativo (ENIAL)</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Encontro Nacional de Inteligência Artificial</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>VIII Encontro Nacional de Inteligência Artificial</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>II Encontro Nacional de Engenharia Biomecânica: ENEBI 2009</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Encontro Nacional de Engenharia Biomecânica</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>III Encontro Nacional de Engenharia Biomecânica</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>III ENCONTRO NACIONAL DE ENSINO DE CIÊNCIAS DA SAÚDE E DO AMBIENTE</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
+      <c r="K123" t="inlineStr"/>
+      <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>Workshop Latinoamericano de Ingeniería de Software Experimental (ESELAW)</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Workshop Iberoamericano de Ingeniería de Requisitos y Ambientes de Software (IDEAS)</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
+      <c r="K124" t="inlineStr"/>
+      <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>International Workshop on Green and Sustainable Software (GREENS)</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>NSF-sponsored workshop on Studying Professional Software Design</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
+      <c r="K125" t="inlineStr"/>
+      <c r="L125" t="inlineStr"/>
+      <c r="M125" t="inlineStr"/>
+      <c r="N125" t="inlineStr"/>
+      <c r="O125" t="inlineStr"/>
+      <c r="P125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>International Workshop on High Performance Computing on Bioinformatics (HPCB)</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>International Workshop on High-Performance Data Management in Grid Environments</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
+      <c r="K126" t="inlineStr"/>
+      <c r="L126" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" t="inlineStr"/>
+      <c r="O126" t="inlineStr"/>
+      <c r="P126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>International Conference on Internet Technologies and Applications (ITA)</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>8th International Conference on Information Technology and Applications (ICITA 2013)</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
+      <c r="K127" t="inlineStr"/>
+      <c r="L127" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="inlineStr"/>
+      <c r="O127" t="inlineStr"/>
+      <c r="P127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>CCI - Latin American Conference on Computational Intelligence (LA-CCI)</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Congresso Ibero-Latino-Americano de Métodos Computacionais em Engenharia (CILAMCE)</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>CILAMCE 2009 : Iberian-Latin-American Congress on Computational Methods in Engineering</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>XXXI Iberian Latin American Congress on Computational Methods in Engineering</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr"/>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
+      <c r="K128" t="inlineStr"/>
+      <c r="L128" t="inlineStr"/>
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" t="inlineStr"/>
+      <c r="O128" t="inlineStr"/>
+      <c r="P128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>IEEE Workshop on Managing Ubiquitous Communications and Services (MUCS)</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Workshop on Many-Task Computing on Grids and Supercomputers (MTAGS)</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
+      <c r="K129" t="inlineStr"/>
+      <c r="L129" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr"/>
+      <c r="O129" t="inlineStr"/>
+      <c r="P129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>International Symposium on Computer Architecture and High Performance Computing Workshop (SBACPADW)</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Computer Architecture and High Performance Computing Workshops (SBAC-PADW), 2010 22nd International Symposium on</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
+      <c r="E130" t="inlineStr"/>
+      <c r="F130" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
+      <c r="K130" t="inlineStr"/>
+      <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr"/>
+      <c r="O130" t="inlineStr"/>
+      <c r="P130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Pesquisa Operacional (SBPO)</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>XL Simpósio Brasileiro de Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Pesquisa Operacional - Prêmio de Iniciação Científica</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>XLIII Simpósio Brasileiro de Pesquisa Operacional - Concurso de Trabalhos de Iniciação Científica</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>XLV Simpósio Brasileiro de Pesquisa Operacional</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
+      <c r="K131" t="inlineStr"/>
+      <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr"/>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>International Workshop on Semantic and Conceptual Issues in Geographic Information Systems (SeCoGIS)</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>International Workshop on Medical Image Analysis and Description for Diagnosis Systems (MIADS) em conjunto com a International Joint Conference on Biomedical Engineering Systems and Technologies (BIOSTEC)</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
+      <c r="E132" t="inlineStr"/>
+      <c r="F132" t="inlineStr"/>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
+      <c r="K132" t="inlineStr"/>
+      <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" t="inlineStr"/>
+      <c r="O132" t="inlineStr"/>
+      <c r="P132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr">
+        <is>
+          <t>Seminário Integrado de Software e Hardware (SEMISH)</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>XL Seminário Integrado de Software e Hardware</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="inlineStr"/>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" t="inlineStr"/>
+      <c r="K133" t="inlineStr"/>
+      <c r="L133" t="inlineStr"/>
+      <c r="M133" t="inlineStr"/>
+      <c r="N133" t="inlineStr"/>
+      <c r="O133" t="inlineStr"/>
+      <c r="P133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="inlineStr">
+        <is>
+          <t>IEEE PES Transmission &amp; Distribution Conference and Exposition Latin America (T&amp;DLA)</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>IEEE PES Transmission and Distribution Conference and Exposition Latin America</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
+      <c r="E134" t="inlineStr"/>
+      <c r="F134" t="inlineStr"/>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" t="inlineStr"/>
+      <c r="I134" t="inlineStr"/>
+      <c r="J134" t="inlineStr"/>
+      <c r="K134" t="inlineStr"/>
+      <c r="L134" t="inlineStr"/>
+      <c r="M134" t="inlineStr"/>
+      <c r="N134" t="inlineStr"/>
+      <c r="O134" t="inlineStr"/>
+      <c r="P134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="inlineStr">
+        <is>
+          <t>Workshop on Applications for Multi-Core Architectures (WAMCA)</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>2012 3rd Workshop on Applications for MultiCore Architectures (WAMCA)</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="inlineStr"/>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
+      <c r="K135" t="inlineStr"/>
+      <c r="L135" t="inlineStr"/>
+      <c r="M135" t="inlineStr"/>
+      <c r="N135" t="inlineStr"/>
+      <c r="O135" t="inlineStr"/>
+      <c r="P135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="inlineStr">
+        <is>
+          <t>International CAD Conference (CAD)</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>the 22nd International ACM Conference</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr"/>
+      <c r="F136" t="inlineStr"/>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" t="inlineStr"/>
+      <c r="K136" t="inlineStr"/>
+      <c r="L136" t="inlineStr"/>
+      <c r="M136" t="inlineStr"/>
+      <c r="N136" t="inlineStr"/>
+      <c r="O136" t="inlineStr"/>
+      <c r="P136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="inlineStr">
+        <is>
+          <t>International Conference on Computer Graphics and Imaging (CGIM)</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>4th International Conference Computer Graphics, Imaging and Visualization</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
+      <c r="E137" t="inlineStr"/>
+      <c r="F137" t="inlineStr"/>
+      <c r="G137" t="inlineStr"/>
+      <c r="H137" t="inlineStr"/>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" t="inlineStr"/>
+      <c r="K137" t="inlineStr"/>
+      <c r="L137" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" t="inlineStr"/>
+      <c r="O137" t="inlineStr"/>
+      <c r="P137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="inlineStr">
+        <is>
+          <t>Workshop de Desafios da Computação Aplicada à Educação (DesafIE)</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Escola Regional de Computação Aplicada à Saúde</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="inlineStr"/>
+      <c r="F138" t="inlineStr"/>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" t="inlineStr"/>
+      <c r="K138" t="inlineStr"/>
+      <c r="L138" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" t="inlineStr"/>
+      <c r="O138" t="inlineStr"/>
+      <c r="P138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="inlineStr">
+        <is>
+          <t>IARIA International Conference on Smart Grids, Green Communications and IT Energy-aware Technologies (ENERGY)</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Third International Conference on Smart Grids, Green Communications and IT Energy-aware Technologies</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="inlineStr"/>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" t="inlineStr"/>
+      <c r="K139" t="inlineStr"/>
+      <c r="L139" t="inlineStr"/>
+      <c r="M139" t="inlineStr"/>
+      <c r="N139" t="inlineStr"/>
+      <c r="O139" t="inlineStr"/>
+      <c r="P139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="inlineStr">
+        <is>
+          <t>International Workshop on Future Internet and Smart Networks (FINS)</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>2º Workshop do testbed FIBRE - Future Internet Brazilian Environment for Experimentation</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" t="inlineStr"/>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
+      <c r="J140" t="inlineStr"/>
+      <c r="K140" t="inlineStr"/>
+      <c r="L140" t="inlineStr"/>
+      <c r="M140" t="inlineStr"/>
+      <c r="N140" t="inlineStr"/>
+      <c r="O140" t="inlineStr"/>
+      <c r="P140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="inlineStr">
+        <is>
+          <t>Workshop on High Performance and Programmable Networking (HPPN)</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>SPIE's Performance and Control of Network Systems II</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="inlineStr"/>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" t="inlineStr"/>
+      <c r="I141" t="inlineStr"/>
+      <c r="J141" t="inlineStr"/>
+      <c r="K141" t="inlineStr"/>
+      <c r="L141" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
+      <c r="N141" t="inlineStr"/>
+      <c r="O141" t="inlineStr"/>
+      <c r="P141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="inlineStr">
+        <is>
+          <t>IARIA International Conference on Networks (ICN)</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>IADIS International Conference on WWW/Internet</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" t="inlineStr"/>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
+      <c r="J142" t="inlineStr"/>
+      <c r="K142" t="inlineStr"/>
+      <c r="L142" t="inlineStr"/>
+      <c r="M142" t="inlineStr"/>
+      <c r="N142" t="inlineStr"/>
+      <c r="O142" t="inlineStr"/>
+      <c r="P142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="inlineStr">
+        <is>
+          <t>International Conference on Internet Computing and Internet of Things (ICOMP)</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>2020 4th Conference on Cloud and Internet of Things (CIoT)</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" t="inlineStr"/>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
+      <c r="J143" t="inlineStr"/>
+      <c r="K143" t="inlineStr"/>
+      <c r="L143" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
+      <c r="N143" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
+      <c r="P143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="inlineStr">
+        <is>
+          <t>International Conference on Human Computer Interaction (INTERACCION)</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>17th International Conference on Human-Computer Interaction (HCI International 2015)</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
+      <c r="J144" t="inlineStr"/>
+      <c r="K144" t="inlineStr"/>
+      <c r="L144" t="inlineStr"/>
+      <c r="M144" t="inlineStr"/>
+      <c r="N144" t="inlineStr"/>
+      <c r="O144" t="inlineStr"/>
+      <c r="P144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="inlineStr">
+        <is>
+          <t>International Workshop on Confluence (IWC)</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>International Workshop on Challenges in e-Science (CIS)</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
+      <c r="E145" t="inlineStr"/>
+      <c r="F145" t="inlineStr"/>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr"/>
+      <c r="I145" t="inlineStr"/>
+      <c r="J145" t="inlineStr"/>
+      <c r="K145" t="inlineStr"/>
+      <c r="L145" t="inlineStr"/>
+      <c r="M145" t="inlineStr"/>
+      <c r="N145" t="inlineStr"/>
+      <c r="O145" t="inlineStr"/>
+      <c r="P145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="inlineStr">
+        <is>
+          <t>Iberchip Workshop (IWS)</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>IEEE Packet Video Workshop</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
+      <c r="J146" t="inlineStr"/>
+      <c r="K146" t="inlineStr"/>
+      <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" t="inlineStr"/>
+      <c r="O146" t="inlineStr"/>
+      <c r="P146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="inlineStr">
+        <is>
+          <t>International Workshop on Science Gateways (IWSG)</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>International Workshop on Scientific Workflows (SWF)</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>International Workshop on the Web and Databases (WebDB)</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>International Workshop on Scientific Workflows, SWF</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>International Workshop on Genomic Databases (IWGD)</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr"/>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" t="inlineStr"/>
+      <c r="I147" t="inlineStr"/>
+      <c r="J147" t="inlineStr"/>
+      <c r="K147" t="inlineStr"/>
+      <c r="L147" t="inlineStr"/>
+      <c r="M147" t="inlineStr"/>
+      <c r="N147" t="inlineStr"/>
+      <c r="O147" t="inlineStr"/>
+      <c r="P147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="inlineStr">
+        <is>
+          <t>Workshop on Logical Reasoning and Computation (LRC)</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Workshop on High Resolution Digital Soil Sensing and Mapping</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" t="inlineStr"/>
+      <c r="K148" t="inlineStr"/>
+      <c r="L148" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
+      <c r="N148" t="inlineStr"/>
+      <c r="O148" t="inlineStr"/>
+      <c r="P148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="inlineStr">
+        <is>
+          <t>Metaheuristics International Conference (MIC)</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>the 18th ACM International Conference</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>the 20th ACM International Conference</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Metaheuristics International Conference</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>10th Metaheuristics International Conference</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
+      <c r="J149" t="inlineStr"/>
+      <c r="K149" t="inlineStr"/>
+      <c r="L149" t="inlineStr"/>
+      <c r="M149" t="inlineStr"/>
+      <c r="N149" t="inlineStr"/>
+      <c r="O149" t="inlineStr"/>
+      <c r="P149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Automação Inteligente (SBAI)</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Simpósio Brasileiro de Telecomunicações e Processamento de Sinais</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>VIII Simpósio Brasileiro de Inteligência Artificial</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>VII Simpósio Brasileiro de Inteligência Artificial</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="inlineStr"/>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="inlineStr"/>
+      <c r="K150" t="inlineStr"/>
+      <c r="L150" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
+      <c r="N150" t="inlineStr"/>
+      <c r="O150" t="inlineStr"/>
+      <c r="P150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="inlineStr">
+        <is>
+          <t>Congresso Brasileiro de Agroinformática (SBIAGRO)</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>13 Congresso da Sociedade Brasleiro de Computação</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>XXI Congresso Brasileiro de Automática</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Segundo Workshop Brasileiro de Bioinformática</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
+      <c r="K151" t="inlineStr"/>
+      <c r="L151" t="inlineStr"/>
+      <c r="M151" t="inlineStr"/>
+      <c r="N151" t="inlineStr"/>
+      <c r="O151" t="inlineStr"/>
+      <c r="P151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="inlineStr">
+        <is>
+          <t>International Conference on Software Engineering Research and Practice (SERP)</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>III Fórum de Educação em Engenharia de Software (FEES), Brazilian Conference on Software: Theory and Practice (CBSoft 2010)</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="inlineStr"/>
+      <c r="K152" t="inlineStr"/>
+      <c r="L152" t="inlineStr"/>
+      <c r="M152" t="inlineStr"/>
+      <c r="N152" t="inlineStr"/>
+      <c r="O152" t="inlineStr"/>
+      <c r="P152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="inlineStr">
+        <is>
+          <t>Asia - Conference on Computer Graphics and Interactive Techniques (SIGGRAPH-Asia)</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>SIGGRAPH Asia 2014 Mobile Graphics and Interactive Applications</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="inlineStr"/>
+      <c r="K153" t="inlineStr"/>
+      <c r="L153" t="inlineStr"/>
+      <c r="M153" t="inlineStr"/>
+      <c r="N153" t="inlineStr"/>
+      <c r="O153" t="inlineStr"/>
+      <c r="P153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="inlineStr">
+        <is>
+          <t>International Workshop on Theory and Practice of Provenance (TaPP)</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>USENIX Workshop on the Theory and Practice of Provenance (TaPP)</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>International Workshop on Theory and Practice of Provenance (TAPP)</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="inlineStr"/>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="inlineStr"/>
+      <c r="K154" t="inlineStr"/>
+      <c r="L154" t="inlineStr"/>
+      <c r="M154" t="inlineStr"/>
+      <c r="N154" t="inlineStr"/>
+      <c r="O154" t="inlineStr"/>
+      <c r="P154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="inlineStr">
+        <is>
+          <t>Congreso Internacional de Informática Educativa (TISE)</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Minicurso da V Escola Regional de Informática RJ/ES</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>XXVI Concurso de Trabalhos de Iniciação Científica</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="inlineStr"/>
+      <c r="K155" t="inlineStr"/>
+      <c r="L155" t="inlineStr"/>
+      <c r="M155" t="inlineStr"/>
+      <c r="N155" t="inlineStr"/>
+      <c r="O155" t="inlineStr"/>
+      <c r="P155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="inlineStr">
+        <is>
+          <t>Workshop on Software Visualization, Evolution and Maintenance (VEM)</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Workshop Brasileiro de Visualização, Evolução e Manutenção de Software (VEM)</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Workshop de Visualização, Manutenção e Evolução de Software (VEM)</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr"/>
+      <c r="I156" t="inlineStr"/>
+      <c r="J156" t="inlineStr"/>
+      <c r="K156" t="inlineStr"/>
+      <c r="L156" t="inlineStr"/>
+      <c r="M156" t="inlineStr"/>
+      <c r="N156" t="inlineStr"/>
+      <c r="O156" t="inlineStr"/>
+      <c r="P156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="inlineStr">
+        <is>
+          <t>Workshop de Desenvolvimento Distribuído de Software (WDES)</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Workshop de Desenvolvimento Baseado em Componentes (WDBC)</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Workshop de Desenvolvimento Distribuído de Software (WDDS), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Workshop de Teses e Dissertações em Qualidade de Software (WTDQS)</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr"/>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="inlineStr"/>
+      <c r="I157" t="inlineStr"/>
+      <c r="J157" t="inlineStr"/>
+      <c r="K157" t="inlineStr"/>
+      <c r="L157" t="inlineStr"/>
+      <c r="M157" t="inlineStr"/>
+      <c r="N157" t="inlineStr"/>
+      <c r="O157" t="inlineStr"/>
+      <c r="P157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="inlineStr">
+        <is>
+          <t>Workshop sobre Ensino de IHC (WEIHC)</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Workshop Brasileiro de e-Science (e-Science)</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>II Workshop Argentino sobre Videojuegos - Wavi 2011</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" t="inlineStr"/>
+      <c r="K158" t="inlineStr"/>
+      <c r="L158" t="inlineStr"/>
+      <c r="M158" t="inlineStr"/>
+      <c r="N158" t="inlineStr"/>
+      <c r="O158" t="inlineStr"/>
+      <c r="P158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="inlineStr">
+        <is>
+          <t>Workshop de Engenharia de Software Baseada em Busca (WESB)</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>XV Workshop de Gerência e Operação de Redes e Serviços</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Workshop de Gerência e Operação de Redes e Serviços</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>XVII Workshop de Gerência e Operação de Redes e Serviços</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Workshop de Manutenção de Software Moderna (WMSWM)</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Workshop de Teses e Dissertações em Engenharia de Software (WTES), Simpósio Brasileiro de Engenharia de Software (SBES)</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" t="inlineStr"/>
+      <c r="K159" t="inlineStr"/>
+      <c r="L159" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
+      <c r="N159" t="inlineStr"/>
+      <c r="O159" t="inlineStr"/>
+      <c r="P159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="inlineStr">
+        <is>
+          <t>Workshop de Ferramentas e Aplicações (WFA)</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Salão de Ferramentas do SBRC</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Segundo Workshop de Grades Computacionais e Aplicações</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Concurso de Teses e Dissertações CTD</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Workshop de Algoritmos e Aplicações em Mineração de Dados</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>XI Workshop de Ferramentas e Aplicações (WFA) - Webmidia 2012</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="inlineStr"/>
+      <c r="K160" t="inlineStr"/>
+      <c r="L160" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
+      <c r="N160" t="inlineStr"/>
+      <c r="O160" t="inlineStr"/>
+      <c r="P160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="inlineStr">
+        <is>
+          <t>Workshop de Redes P2P, Dinâmicas, Sociais e Orientadas a Conteúdo (WP2P+)</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Workshop de Redes Dinamicas e Sistemas Peer-to-Peer (WP2P)</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
+      <c r="E161" t="inlineStr"/>
+      <c r="F161" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
+      <c r="J161" t="inlineStr"/>
+      <c r="K161" t="inlineStr"/>
+      <c r="L161" t="inlineStr"/>
+      <c r="M161" t="inlineStr"/>
+      <c r="N161" t="inlineStr"/>
+      <c r="O161" t="inlineStr"/>
+      <c r="P161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="inlineStr">
+        <is>
+          <t>Workshop de Software Livre (WSL)</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Workshop on Software Reuse Efforts (WSRE)</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="inlineStr"/>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" t="inlineStr"/>
+      <c r="I162" t="inlineStr"/>
+      <c r="J162" t="inlineStr"/>
+      <c r="K162" t="inlineStr"/>
+      <c r="L162" t="inlineStr"/>
+      <c r="M162" t="inlineStr"/>
+      <c r="N162" t="inlineStr"/>
+      <c r="O162" t="inlineStr"/>
+      <c r="P162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="inlineStr">
+        <is>
+          <t>Workshop de Testes e Tolerância a Falhas (WTF)</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Workshop de Teses e Dissertações do CBSoft (WTDSoft)</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Workshop de Teses e Dissertações em Banco de Dados (WTDBD)</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Concurso de Teses e Dissertações da SBC (CTD)</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
+      <c r="J163" t="inlineStr"/>
+      <c r="K163" t="inlineStr"/>
+      <c r="L163" t="inlineStr"/>
+      <c r="M163" t="inlineStr"/>
+      <c r="N163" t="inlineStr"/>
+      <c r="O163" t="inlineStr"/>
+      <c r="P163" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>